<commit_message>
Added Dimension Model Description
</commit_message>
<xml_diff>
--- a/Documentation/DataSources.xlsx
+++ b/Documentation/DataSources.xlsx
@@ -5,20 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinee_000\OneDrive\Vineet\Courses\Data Warehouse &amp; Business Intelligence\Project\DI Project\student_behavior_di\Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinee_000\OneDrive\Vineet\Courses\Data Warehouse &amp; Business Intelligence\Project\DI Project\student_behavior_di\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" tabRatio="638" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
-    <sheet name="Student_Behavior_SE_SW" sheetId="2" r:id="rId2"/>
-    <sheet name="Student_Behavior_NE" sheetId="3" r:id="rId3"/>
-    <sheet name="Student_Behavior_NW" sheetId="4" r:id="rId4"/>
-    <sheet name="Student_Behavior_AL" sheetId="5" r:id="rId5"/>
-    <sheet name="XML" sheetId="6" r:id="rId6"/>
-    <sheet name="Text" sheetId="7" r:id="rId7"/>
+    <sheet name="Student_Behavior" sheetId="8" r:id="rId2"/>
+    <sheet name="XML" sheetId="6" r:id="rId3"/>
+    <sheet name="Text" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="165">
   <si>
     <t>Student_Behavior_SE_SW</t>
   </si>
@@ -524,6 +521,9 @@
   </si>
   <si>
     <t>Behavior_Role_Desc</t>
+  </si>
+  <si>
+    <t>grade_level</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -596,8 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,37 +1085,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.21875" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.21875" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.109375" customWidth="1"/>
+    <col min="16" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="E1" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="I1" s="5" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="P1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1128,7 +1149,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>38</v>
@@ -1137,16 +1158,27 @@
         <v>10</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="6"/>
+      <c r="P2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
@@ -1155,23 +1187,36 @@
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="6">
-        <v>10</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="6">
+        <v>6</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
@@ -1182,25 +1227,36 @@
         <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="P4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>45</v>
       </c>
@@ -1211,23 +1267,38 @@
         <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="G5" s="6">
+        <v>10</v>
+      </c>
       <c r="I5" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="6">
+        <v>5</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>46</v>
       </c>
@@ -1238,23 +1309,36 @@
         <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="G6" s="6">
+        <v>19</v>
+      </c>
       <c r="I6" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="6"/>
+      <c r="L6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="P6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>47</v>
       </c>
@@ -1265,7 +1349,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>38</v>
@@ -1274,16 +1358,27 @@
         <v>10</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="6"/>
+      <c r="L7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="P7" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>48</v>
       </c>
@@ -1293,17 +1388,37 @@
       <c r="C8" s="6">
         <v>10</v>
       </c>
+      <c r="E8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="6">
+        <v>10</v>
+      </c>
       <c r="I8" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="P8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>49</v>
       </c>
@@ -1313,17 +1428,37 @@
       <c r="C9" s="6">
         <v>10</v>
       </c>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="6">
+        <v>10</v>
+      </c>
       <c r="I9" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="P9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>50</v>
       </c>
@@ -1333,17 +1468,37 @@
       <c r="C10" s="6">
         <v>10</v>
       </c>
+      <c r="E10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="6">
+        <v>10</v>
+      </c>
       <c r="I10" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="P10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>51</v>
       </c>
@@ -1353,17 +1508,37 @@
       <c r="C11" s="6">
         <v>10</v>
       </c>
+      <c r="E11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="6">
+        <v>10</v>
+      </c>
       <c r="I11" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="P11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>52</v>
       </c>
@@ -1373,47 +1548,105 @@
       <c r="C12" s="6">
         <v>1</v>
       </c>
+      <c r="E12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
       <c r="I12" s="6" t="s">
         <v>52</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="E15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="P12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="I15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="I14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="P14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="6">
+        <v>10</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="P15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>38</v>
@@ -1422,7 +1655,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>38</v>
@@ -1436,1224 +1669,698 @@
       <c r="J16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="P16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="6">
+        <v>5</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="P17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="E17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="6">
-        <v>10</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="6" t="s">
+      <c r="C18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="6">
-        <v>10</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="6">
-        <v>5</v>
-      </c>
+      <c r="G18" s="6"/>
       <c r="I18" s="6" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K18" s="6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" s="6">
+        <v>6</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="6">
-        <v>10</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="6"/>
       <c r="I19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="6">
+        <v>6</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="6">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="6">
+        <v>10</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="P20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="I22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="P22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="6"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="6">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="6">
+        <v>10</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="P23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N24" s="6">
+        <v>6</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="6">
+        <v>19</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="6">
+        <v>19</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="P25" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K19" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="6">
-        <v>19</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="I20" s="6" t="s">
+      <c r="C26" s="6">
+        <v>10</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="6">
+        <v>10</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="P26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="6">
-        <v>10</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="6">
-        <v>10</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="B27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="6">
+        <v>10</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N27" s="6">
+        <v>5</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K21" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="6">
-        <v>10</v>
-      </c>
-      <c r="I22" s="6" t="s">
+      <c r="B28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="6">
+        <v>10</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="6">
+        <v>10</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N28" s="6">
+        <v>5</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K22" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="6">
-        <v>10</v>
-      </c>
-      <c r="I23" s="6" t="s">
+      <c r="B29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="6">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="6">
+        <v>10</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N29" s="6">
+        <v>5</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="6">
-        <v>10</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="B30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="6">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="6">
+        <v>10</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="P30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="6">
-        <v>10</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="B31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="6">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="6">
+        <v>10</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N31" s="6"/>
+      <c r="P31" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K25" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="B32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="6">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="6">
+        <v>10</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N32" s="6"/>
+      <c r="P32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6" t="s">
+      <c r="B33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="6">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I27" s="6" t="s">
+      <c r="F33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="6">
+        <v>10</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N33" s="6"/>
+      <c r="P33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="6">
-        <v>10</v>
+      <c r="B34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="6">
+        <v>10</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="6">
+        <v>10</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N34" s="6"/>
+      <c r="P34" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="I1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="I2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="E3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="I4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="I5" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="I8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="I9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="I10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="I11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="I12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="I1" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="I2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="6">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="I4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="6">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="6">
-        <v>6</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="6">
-        <v>6</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K6" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="I8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K8" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="I9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="I10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="I11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="I12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="D1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="G1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3087,12 +2794,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3258,10 +2965,27 @@
       <c r="C11">
         <v>10</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>